<commit_message>
Atualização de bases das ligas, do dia: 02-05-2024 às 20:28
</commit_message>
<xml_diff>
--- a/Argentina Nacional B/Argentina Nacional B.xlsx
+++ b/Argentina Nacional B/Argentina Nacional B.xlsx
@@ -97,10 +97,10 @@
     <t>PL_AhUnder</t>
   </si>
   <si>
-    <t>7698812</t>
+    <t>7698813</t>
   </si>
   <si>
-    <t>7698813</t>
+    <t>7698812</t>
   </si>
   <si>
     <t>7698816</t>
@@ -124,7 +124,7 @@
     <t>7698806</t>
   </si>
   <si>
-    <t>8165223</t>
+    <t>8165224</t>
   </si>
   <si>
     <t>7698810</t>
@@ -142,7 +142,7 @@
     <t>8165210</t>
   </si>
   <si>
-    <t>8165224</t>
+    <t>8165223</t>
   </si>
   <si>
     <t>7698585</t>
@@ -4268,7 +4268,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>6150859</v>
+        <v>6150461</v>
       </c>
       <c r="C43" t="s">
         <v>45</v>
@@ -4277,76 +4277,76 @@
         <v>45096.625</v>
       </c>
       <c r="E43" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="F43" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J43">
-        <v>2.375</v>
+        <v>2.1</v>
       </c>
       <c r="K43">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="L43">
-        <v>2.625</v>
+        <v>3.3</v>
       </c>
       <c r="M43">
-        <v>1.909</v>
+        <v>2.25</v>
       </c>
       <c r="N43">
         <v>3.1</v>
       </c>
       <c r="O43">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="P43">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="Q43">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="R43">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="S43">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T43">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="U43">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V43">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="W43">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="X43">
         <v>-1</v>
       </c>
       <c r="Y43">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z43">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA43">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB43">
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="44" spans="1:28">
@@ -4354,7 +4354,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>6150461</v>
+        <v>6150859</v>
       </c>
       <c r="C44" t="s">
         <v>45</v>
@@ -4363,76 +4363,76 @@
         <v>45096.625</v>
       </c>
       <c r="E44" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F44" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J44">
-        <v>2.1</v>
+        <v>2.375</v>
       </c>
       <c r="K44">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="L44">
-        <v>3.3</v>
+        <v>2.625</v>
       </c>
       <c r="M44">
-        <v>2.25</v>
+        <v>1.909</v>
       </c>
       <c r="N44">
         <v>3.1</v>
       </c>
       <c r="O44">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="P44">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q44">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="R44">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="S44">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="T44">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="U44">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V44">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="W44">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="X44">
         <v>-1</v>
       </c>
       <c r="Y44">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="Z44">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA44">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB44">
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:28">
@@ -5644,7 +5644,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>6150463</v>
+        <v>6150861</v>
       </c>
       <c r="C59" t="s">
         <v>45</v>
@@ -5653,46 +5653,46 @@
         <v>45102.625</v>
       </c>
       <c r="E59" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F59" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J59">
-        <v>2.55</v>
+        <v>2.15</v>
       </c>
       <c r="K59">
-        <v>2.55</v>
+        <v>2.9</v>
       </c>
       <c r="L59">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="M59">
-        <v>2.55</v>
+        <v>2.1</v>
       </c>
       <c r="N59">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="O59">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="P59">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="Q59">
-        <v>1.725</v>
+        <v>1.75</v>
       </c>
       <c r="R59">
-        <v>2.075</v>
+        <v>2.05</v>
       </c>
       <c r="S59">
         <v>2</v>
@@ -5707,16 +5707,16 @@
         <v>-1</v>
       </c>
       <c r="W59">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="X59">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="Y59">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="Z59">
-        <v>1.075</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AA59">
         <v>0</v>
@@ -5730,7 +5730,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>6150861</v>
+        <v>6150463</v>
       </c>
       <c r="C60" t="s">
         <v>45</v>
@@ -5739,46 +5739,46 @@
         <v>45102.625</v>
       </c>
       <c r="E60" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="F60" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I60" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J60">
-        <v>2.15</v>
+        <v>2.55</v>
       </c>
       <c r="K60">
-        <v>2.9</v>
+        <v>2.55</v>
       </c>
       <c r="L60">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="M60">
-        <v>2.1</v>
+        <v>2.55</v>
       </c>
       <c r="N60">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="O60">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="P60">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q60">
-        <v>1.75</v>
+        <v>1.725</v>
       </c>
       <c r="R60">
-        <v>2.05</v>
+        <v>2.075</v>
       </c>
       <c r="S60">
         <v>2</v>
@@ -5793,16 +5793,16 @@
         <v>-1</v>
       </c>
       <c r="W60">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="X60">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="Y60">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z60">
-        <v>0.5249999999999999</v>
+        <v>1.075</v>
       </c>
       <c r="AA60">
         <v>0</v>
@@ -7192,7 +7192,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>6150697</v>
+        <v>6150467</v>
       </c>
       <c r="C77" t="s">
         <v>45</v>
@@ -7201,58 +7201,58 @@
         <v>45109.70833333334</v>
       </c>
       <c r="E77" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F77" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="G77">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77" t="s">
         <v>88</v>
       </c>
       <c r="J77">
-        <v>2</v>
+        <v>2.2</v>
       </c>
       <c r="K77">
-        <v>3.1</v>
+        <v>2.75</v>
       </c>
       <c r="L77">
         <v>3.5</v>
       </c>
       <c r="M77">
-        <v>1.666</v>
+        <v>2</v>
       </c>
       <c r="N77">
-        <v>3.6</v>
+        <v>2.875</v>
       </c>
       <c r="O77">
-        <v>5.5</v>
+        <v>4.75</v>
       </c>
       <c r="P77">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="Q77">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="R77">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="S77">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T77">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="U77">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="V77">
-        <v>0.6659999999999999</v>
+        <v>1</v>
       </c>
       <c r="W77">
         <v>-1</v>
@@ -7261,16 +7261,16 @@
         <v>-1</v>
       </c>
       <c r="Y77">
-        <v>0.875</v>
+        <v>1.025</v>
       </c>
       <c r="Z77">
         <v>-1</v>
       </c>
       <c r="AA77">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB77">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="78" spans="1:28">
@@ -7278,7 +7278,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>6150467</v>
+        <v>6150697</v>
       </c>
       <c r="C78" t="s">
         <v>45</v>
@@ -7287,58 +7287,58 @@
         <v>45109.70833333334</v>
       </c>
       <c r="E78" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F78" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I78" t="s">
         <v>88</v>
       </c>
       <c r="J78">
-        <v>2.2</v>
+        <v>2</v>
       </c>
       <c r="K78">
-        <v>2.75</v>
+        <v>3.1</v>
       </c>
       <c r="L78">
         <v>3.5</v>
       </c>
       <c r="M78">
-        <v>2</v>
+        <v>1.666</v>
       </c>
       <c r="N78">
-        <v>2.875</v>
+        <v>3.6</v>
       </c>
       <c r="O78">
-        <v>4.75</v>
+        <v>5.5</v>
       </c>
       <c r="P78">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="Q78">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="R78">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="S78">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="T78">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="U78">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V78">
-        <v>1</v>
+        <v>0.6659999999999999</v>
       </c>
       <c r="W78">
         <v>-1</v>
@@ -7347,16 +7347,16 @@
         <v>-1</v>
       </c>
       <c r="Y78">
-        <v>1.025</v>
+        <v>0.875</v>
       </c>
       <c r="Z78">
         <v>-1</v>
       </c>
       <c r="AA78">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AB78">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="79" spans="1:28">
@@ -8138,7 +8138,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>6150704</v>
+        <v>6870444</v>
       </c>
       <c r="C88" t="s">
         <v>45</v>
@@ -8147,10 +8147,10 @@
         <v>45115.64583333334</v>
       </c>
       <c r="E88" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="F88" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -8162,40 +8162,40 @@
         <v>90</v>
       </c>
       <c r="J88">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
       <c r="K88">
         <v>2.875</v>
       </c>
       <c r="L88">
-        <v>2.875</v>
+        <v>2.375</v>
       </c>
       <c r="M88">
-        <v>2.5</v>
+        <v>3.3</v>
       </c>
       <c r="N88">
-        <v>2.875</v>
+        <v>3</v>
       </c>
       <c r="O88">
-        <v>3.3</v>
+        <v>2.375</v>
       </c>
       <c r="P88">
-        <v>-0.25</v>
+        <v>0.25</v>
       </c>
       <c r="Q88">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="R88">
-        <v>1.75</v>
+        <v>1.975</v>
       </c>
       <c r="S88">
         <v>2</v>
       </c>
       <c r="T88">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="U88">
-        <v>1.775</v>
+        <v>1.925</v>
       </c>
       <c r="V88">
         <v>-1</v>
@@ -8204,13 +8204,13 @@
         <v>-1</v>
       </c>
       <c r="X88">
-        <v>2.3</v>
+        <v>1.375</v>
       </c>
       <c r="Y88">
         <v>-1</v>
       </c>
       <c r="Z88">
-        <v>0.75</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA88">
         <v>0</v>
@@ -8224,7 +8224,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>6870414</v>
+        <v>6150704</v>
       </c>
       <c r="C89" t="s">
         <v>45</v>
@@ -8233,55 +8233,55 @@
         <v>45115.64583333334</v>
       </c>
       <c r="E89" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="F89" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G89">
         <v>0</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I89" t="s">
         <v>90</v>
       </c>
       <c r="J89">
-        <v>2.15</v>
+        <v>2.4</v>
       </c>
       <c r="K89">
-        <v>2.9</v>
+        <v>2.875</v>
       </c>
       <c r="L89">
+        <v>2.875</v>
+      </c>
+      <c r="M89">
+        <v>2.5</v>
+      </c>
+      <c r="N89">
+        <v>2.875</v>
+      </c>
+      <c r="O89">
         <v>3.3</v>
-      </c>
-      <c r="M89">
-        <v>2.25</v>
-      </c>
-      <c r="N89">
-        <v>3</v>
-      </c>
-      <c r="O89">
-        <v>3.6</v>
       </c>
       <c r="P89">
         <v>-0.25</v>
       </c>
       <c r="Q89">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="R89">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="S89">
         <v>2</v>
       </c>
       <c r="T89">
-        <v>1.8</v>
+        <v>2.025</v>
       </c>
       <c r="U89">
-        <v>2</v>
+        <v>1.775</v>
       </c>
       <c r="V89">
         <v>-1</v>
@@ -8290,19 +8290,19 @@
         <v>-1</v>
       </c>
       <c r="X89">
-        <v>2.6</v>
+        <v>2.3</v>
       </c>
       <c r="Y89">
         <v>-1</v>
       </c>
       <c r="Z89">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
       <c r="AA89">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB89">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:28">
@@ -8310,7 +8310,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>6870444</v>
+        <v>6870414</v>
       </c>
       <c r="C90" t="s">
         <v>45</v>
@@ -8319,55 +8319,55 @@
         <v>45115.64583333334</v>
       </c>
       <c r="E90" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F90" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="G90">
         <v>0</v>
       </c>
       <c r="H90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I90" t="s">
         <v>90</v>
       </c>
       <c r="J90">
+        <v>2.15</v>
+      </c>
+      <c r="K90">
         <v>2.9</v>
       </c>
-      <c r="K90">
-        <v>2.875</v>
-      </c>
       <c r="L90">
-        <v>2.375</v>
+        <v>3.3</v>
       </c>
       <c r="M90">
-        <v>3.3</v>
+        <v>2.25</v>
       </c>
       <c r="N90">
         <v>3</v>
       </c>
       <c r="O90">
-        <v>2.375</v>
+        <v>3.6</v>
       </c>
       <c r="P90">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="Q90">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="R90">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="S90">
         <v>2</v>
       </c>
       <c r="T90">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="U90">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V90">
         <v>-1</v>
@@ -8376,19 +8376,19 @@
         <v>-1</v>
       </c>
       <c r="X90">
-        <v>1.375</v>
+        <v>2.6</v>
       </c>
       <c r="Y90">
         <v>-1</v>
       </c>
       <c r="Z90">
-        <v>0.9750000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="AA90">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:28">
@@ -22414,7 +22414,7 @@
         <v>252</v>
       </c>
       <c r="B254">
-        <v>6150931</v>
+        <v>6264156</v>
       </c>
       <c r="C254" t="s">
         <v>45</v>
@@ -22423,13 +22423,13 @@
         <v>45185.64583333334</v>
       </c>
       <c r="E254" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F254" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="G254">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H254">
         <v>0</v>
@@ -22438,43 +22438,43 @@
         <v>88</v>
       </c>
       <c r="J254">
-        <v>1.5</v>
+        <v>2.75</v>
       </c>
       <c r="K254">
-        <v>4</v>
+        <v>2.75</v>
       </c>
       <c r="L254">
-        <v>5</v>
+        <v>2.625</v>
       </c>
       <c r="M254">
-        <v>1.363</v>
+        <v>2.25</v>
       </c>
       <c r="N254">
-        <v>4.5</v>
+        <v>2.875</v>
       </c>
       <c r="O254">
-        <v>10</v>
+        <v>3.75</v>
       </c>
       <c r="P254">
-        <v>-1.25</v>
+        <v>-0.25</v>
       </c>
       <c r="Q254">
+        <v>1.95</v>
+      </c>
+      <c r="R254">
         <v>1.85</v>
       </c>
-      <c r="R254">
+      <c r="S254">
+        <v>1.75</v>
+      </c>
+      <c r="T254">
+        <v>1.85</v>
+      </c>
+      <c r="U254">
         <v>1.95</v>
       </c>
-      <c r="S254">
-        <v>2.25</v>
-      </c>
-      <c r="T254">
-        <v>1.825</v>
-      </c>
-      <c r="U254">
-        <v>1.975</v>
-      </c>
       <c r="V254">
-        <v>0.363</v>
+        <v>1.25</v>
       </c>
       <c r="W254">
         <v>-1</v>
@@ -22483,16 +22483,16 @@
         <v>-1</v>
       </c>
       <c r="Y254">
-        <v>0.8500000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="Z254">
         <v>-1</v>
       </c>
       <c r="AA254">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB254">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="255" spans="1:28">
@@ -22500,7 +22500,7 @@
         <v>253</v>
       </c>
       <c r="B255">
-        <v>6264156</v>
+        <v>6150931</v>
       </c>
       <c r="C255" t="s">
         <v>45</v>
@@ -22509,13 +22509,13 @@
         <v>45185.64583333334</v>
       </c>
       <c r="E255" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F255" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="G255">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H255">
         <v>0</v>
@@ -22524,43 +22524,43 @@
         <v>88</v>
       </c>
       <c r="J255">
-        <v>2.75</v>
+        <v>1.5</v>
       </c>
       <c r="K255">
-        <v>2.75</v>
+        <v>4</v>
       </c>
       <c r="L255">
-        <v>2.625</v>
+        <v>5</v>
       </c>
       <c r="M255">
+        <v>1.363</v>
+      </c>
+      <c r="N255">
+        <v>4.5</v>
+      </c>
+      <c r="O255">
+        <v>10</v>
+      </c>
+      <c r="P255">
+        <v>-1.25</v>
+      </c>
+      <c r="Q255">
+        <v>1.85</v>
+      </c>
+      <c r="R255">
+        <v>1.95</v>
+      </c>
+      <c r="S255">
         <v>2.25</v>
       </c>
-      <c r="N255">
-        <v>2.875</v>
-      </c>
-      <c r="O255">
-        <v>3.75</v>
-      </c>
-      <c r="P255">
-        <v>-0.25</v>
-      </c>
-      <c r="Q255">
-        <v>1.95</v>
-      </c>
-      <c r="R255">
-        <v>1.85</v>
-      </c>
-      <c r="S255">
-        <v>1.75</v>
-      </c>
       <c r="T255">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="U255">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V255">
-        <v>1.25</v>
+        <v>0.363</v>
       </c>
       <c r="W255">
         <v>-1</v>
@@ -22569,16 +22569,16 @@
         <v>-1</v>
       </c>
       <c r="Y255">
-        <v>0.95</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z255">
         <v>-1</v>
       </c>
       <c r="AA255">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB255">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="256" spans="1:28">
@@ -23446,7 +23446,7 @@
         <v>264</v>
       </c>
       <c r="B266">
-        <v>6256581</v>
+        <v>6150576</v>
       </c>
       <c r="C266" t="s">
         <v>45</v>
@@ -23455,76 +23455,76 @@
         <v>45186.75</v>
       </c>
       <c r="E266" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="F266" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G266">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H266">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I266" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J266">
-        <v>2.1</v>
+        <v>1.909</v>
       </c>
       <c r="K266">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="L266">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M266">
-        <v>1.75</v>
+        <v>1.727</v>
       </c>
       <c r="N266">
-        <v>3.75</v>
+        <v>3.3</v>
       </c>
       <c r="O266">
-        <v>4.5</v>
+        <v>5.75</v>
       </c>
       <c r="P266">
         <v>-0.75</v>
       </c>
       <c r="Q266">
+        <v>2</v>
+      </c>
+      <c r="R266">
+        <v>1.8</v>
+      </c>
+      <c r="S266">
+        <v>2</v>
+      </c>
+      <c r="T266">
         <v>1.925</v>
       </c>
-      <c r="R266">
+      <c r="U266">
         <v>1.875</v>
       </c>
-      <c r="S266">
-        <v>2.25</v>
-      </c>
-      <c r="T266">
-        <v>1.9</v>
-      </c>
-      <c r="U266">
-        <v>1.9</v>
-      </c>
       <c r="V266">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="W266">
         <v>-1</v>
       </c>
       <c r="X266">
-        <v>-1</v>
+        <v>4.75</v>
       </c>
       <c r="Y266">
+        <v>-1</v>
+      </c>
+      <c r="Z266">
+        <v>0.8</v>
+      </c>
+      <c r="AA266">
         <v>0.925</v>
       </c>
-      <c r="Z266">
-        <v>-1</v>
-      </c>
-      <c r="AA266">
-        <v>-0.5</v>
-      </c>
       <c r="AB266">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="267" spans="1:28">
@@ -23532,7 +23532,7 @@
         <v>265</v>
       </c>
       <c r="B267">
-        <v>6150576</v>
+        <v>6256581</v>
       </c>
       <c r="C267" t="s">
         <v>45</v>
@@ -23541,76 +23541,76 @@
         <v>45186.75</v>
       </c>
       <c r="E267" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="F267" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G267">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H267">
+        <v>0</v>
+      </c>
+      <c r="I267" t="s">
+        <v>88</v>
+      </c>
+      <c r="J267">
+        <v>2.1</v>
+      </c>
+      <c r="K267">
+        <v>3.25</v>
+      </c>
+      <c r="L267">
         <v>3</v>
       </c>
-      <c r="I267" t="s">
-        <v>90</v>
-      </c>
-      <c r="J267">
-        <v>1.909</v>
-      </c>
-      <c r="K267">
-        <v>3</v>
-      </c>
-      <c r="L267">
-        <v>4</v>
-      </c>
       <c r="M267">
-        <v>1.727</v>
+        <v>1.75</v>
       </c>
       <c r="N267">
-        <v>3.3</v>
+        <v>3.75</v>
       </c>
       <c r="O267">
-        <v>5.75</v>
+        <v>4.5</v>
       </c>
       <c r="P267">
         <v>-0.75</v>
       </c>
       <c r="Q267">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="R267">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="S267">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="T267">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="U267">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="V267">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="W267">
         <v>-1</v>
       </c>
       <c r="X267">
-        <v>4.75</v>
+        <v>-1</v>
       </c>
       <c r="Y267">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="Z267">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA267">
-        <v>0.925</v>
+        <v>-0.5</v>
       </c>
       <c r="AB267">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="268" spans="1:28">
@@ -25768,7 +25768,7 @@
         <v>291</v>
       </c>
       <c r="B293">
-        <v>6327517</v>
+        <v>6290533</v>
       </c>
       <c r="C293" t="s">
         <v>45</v>
@@ -25777,76 +25777,76 @@
         <v>45199.64583333334</v>
       </c>
       <c r="E293" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F293" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G293">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H293">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I293" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J293">
-        <v>2.375</v>
+        <v>2</v>
       </c>
       <c r="K293">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="L293">
+        <v>3.6</v>
+      </c>
+      <c r="M293">
+        <v>2.25</v>
+      </c>
+      <c r="N293">
         <v>3</v>
       </c>
-      <c r="M293">
-        <v>2.5</v>
-      </c>
-      <c r="N293">
-        <v>2.9</v>
-      </c>
       <c r="O293">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="P293">
         <v>-0.25</v>
       </c>
       <c r="Q293">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="R293">
-        <v>1.75</v>
+        <v>1.875</v>
       </c>
       <c r="S293">
         <v>2</v>
       </c>
       <c r="T293">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="U293">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="V293">
-        <v>1.5</v>
+        <v>-1</v>
       </c>
       <c r="W293">
         <v>-1</v>
       </c>
       <c r="X293">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Y293">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z293">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AA293">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB293">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="294" spans="1:28">
@@ -25854,7 +25854,7 @@
         <v>292</v>
       </c>
       <c r="B294">
-        <v>6290533</v>
+        <v>6327517</v>
       </c>
       <c r="C294" t="s">
         <v>45</v>
@@ -25863,76 +25863,76 @@
         <v>45199.64583333334</v>
       </c>
       <c r="E294" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F294" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G294">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H294">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I294" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J294">
-        <v>2</v>
+        <v>2.375</v>
       </c>
       <c r="K294">
+        <v>2.9</v>
+      </c>
+      <c r="L294">
         <v>3</v>
       </c>
-      <c r="L294">
-        <v>3.6</v>
-      </c>
       <c r="M294">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="N294">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="O294">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="P294">
         <v>-0.25</v>
       </c>
       <c r="Q294">
-        <v>1.925</v>
+        <v>2.05</v>
       </c>
       <c r="R294">
-        <v>1.875</v>
+        <v>1.75</v>
       </c>
       <c r="S294">
         <v>2</v>
       </c>
       <c r="T294">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="U294">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="V294">
-        <v>-1</v>
+        <v>1.5</v>
       </c>
       <c r="W294">
         <v>-1</v>
       </c>
       <c r="X294">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y294">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z294">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AA294">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB294">
-        <v>0.8999999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:28">
@@ -28606,7 +28606,7 @@
         <v>324</v>
       </c>
       <c r="B326">
-        <v>6356449</v>
+        <v>6360015</v>
       </c>
       <c r="C326" t="s">
         <v>45</v>
@@ -28615,19 +28615,19 @@
         <v>45214.64583333334</v>
       </c>
       <c r="E326" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F326" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G326">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H326">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I326" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J326">
         <v>1.8</v>
@@ -28645,46 +28645,46 @@
         <v>3.1</v>
       </c>
       <c r="O326">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="P326">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q326">
-        <v>1.775</v>
+        <v>2.05</v>
       </c>
       <c r="R326">
-        <v>2.025</v>
+        <v>1.8</v>
       </c>
       <c r="S326">
         <v>2.25</v>
       </c>
       <c r="T326">
-        <v>1.925</v>
+        <v>2.1</v>
       </c>
       <c r="U326">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="V326">
         <v>-1</v>
       </c>
       <c r="W326">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="X326">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y326">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z326">
-        <v>0.5125</v>
+        <v>0.8</v>
       </c>
       <c r="AA326">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="AB326">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="327" spans="1:28">
@@ -28778,7 +28778,7 @@
         <v>326</v>
       </c>
       <c r="B328">
-        <v>6360015</v>
+        <v>6356449</v>
       </c>
       <c r="C328" t="s">
         <v>45</v>
@@ -28787,19 +28787,19 @@
         <v>45214.64583333334</v>
       </c>
       <c r="E328" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F328" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G328">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H328">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I328" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J328">
         <v>1.8</v>
@@ -28817,46 +28817,46 @@
         <v>3.1</v>
       </c>
       <c r="O328">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="P328">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="Q328">
-        <v>2.05</v>
+        <v>1.775</v>
       </c>
       <c r="R328">
-        <v>1.8</v>
+        <v>2.025</v>
       </c>
       <c r="S328">
         <v>2.25</v>
       </c>
       <c r="T328">
+        <v>1.925</v>
+      </c>
+      <c r="U328">
+        <v>1.875</v>
+      </c>
+      <c r="V328">
+        <v>-1</v>
+      </c>
+      <c r="W328">
         <v>2.1</v>
       </c>
-      <c r="U328">
-        <v>1.775</v>
-      </c>
-      <c r="V328">
-        <v>-1</v>
-      </c>
-      <c r="W328">
-        <v>-1</v>
-      </c>
       <c r="X328">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y328">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="Z328">
-        <v>0.8</v>
+        <v>0.5125</v>
       </c>
       <c r="AA328">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="AB328">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="329" spans="1:28">
@@ -28864,7 +28864,7 @@
         <v>327</v>
       </c>
       <c r="B329">
-        <v>7323531</v>
+        <v>7323530</v>
       </c>
       <c r="C329" t="s">
         <v>45</v>
@@ -28873,76 +28873,76 @@
         <v>45214.64583333334</v>
       </c>
       <c r="E329" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F329" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="G329">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H329">
         <v>1</v>
       </c>
       <c r="I329" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J329">
-        <v>2.75</v>
+        <v>1.8</v>
       </c>
       <c r="K329">
         <v>3.2</v>
       </c>
       <c r="L329">
-        <v>2.375</v>
+        <v>4</v>
       </c>
       <c r="M329">
-        <v>4.333</v>
+        <v>1.65</v>
       </c>
       <c r="N329">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="O329">
-        <v>1.95</v>
+        <v>6.5</v>
       </c>
       <c r="P329">
-        <v>0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="Q329">
-        <v>1.825</v>
+        <v>1.775</v>
       </c>
       <c r="R329">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="S329">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="T329">
-        <v>1.975</v>
+        <v>1.775</v>
       </c>
       <c r="U329">
-        <v>1.825</v>
+        <v>2.025</v>
       </c>
       <c r="V329">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="W329">
-        <v>2.25</v>
+        <v>-1</v>
       </c>
       <c r="X329">
         <v>-1</v>
       </c>
       <c r="Y329">
-        <v>0.825</v>
+        <v>0.3875</v>
       </c>
       <c r="Z329">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AA329">
-        <v>-0.5</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB329">
-        <v>0.4125</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="330" spans="1:28">
@@ -28950,7 +28950,7 @@
         <v>328</v>
       </c>
       <c r="B330">
-        <v>7323533</v>
+        <v>7323531</v>
       </c>
       <c r="C330" t="s">
         <v>45</v>
@@ -28959,76 +28959,76 @@
         <v>45214.64583333334</v>
       </c>
       <c r="E330" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F330" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G330">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H330">
         <v>1</v>
       </c>
       <c r="I330" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J330">
-        <v>2.2</v>
+        <v>2.75</v>
       </c>
       <c r="K330">
         <v>3.2</v>
       </c>
       <c r="L330">
-        <v>3</v>
+        <v>2.375</v>
       </c>
       <c r="M330">
-        <v>3</v>
+        <v>4.333</v>
       </c>
       <c r="N330">
-        <v>3.1</v>
+        <v>3.25</v>
       </c>
       <c r="O330">
-        <v>2.55</v>
+        <v>1.95</v>
       </c>
       <c r="P330">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q330">
-        <v>2.125</v>
+        <v>1.825</v>
       </c>
       <c r="R330">
-        <v>1.75</v>
+        <v>1.975</v>
       </c>
       <c r="S330">
         <v>2.25</v>
       </c>
       <c r="T330">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="U330">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="V330">
         <v>-1</v>
       </c>
       <c r="W330">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="X330">
-        <v>1.55</v>
+        <v>-1</v>
       </c>
       <c r="Y330">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z330">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AA330">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB330">
-        <v>0.8</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="331" spans="1:28">
@@ -29122,7 +29122,7 @@
         <v>330</v>
       </c>
       <c r="B332">
-        <v>7323530</v>
+        <v>7323533</v>
       </c>
       <c r="C332" t="s">
         <v>45</v>
@@ -29131,76 +29131,76 @@
         <v>45214.64583333334</v>
       </c>
       <c r="E332" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F332" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G332">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H332">
         <v>1</v>
       </c>
       <c r="I332" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J332">
-        <v>1.8</v>
+        <v>2.2</v>
       </c>
       <c r="K332">
         <v>3.2</v>
       </c>
       <c r="L332">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M332">
-        <v>1.65</v>
+        <v>3</v>
       </c>
       <c r="N332">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="O332">
-        <v>6.5</v>
+        <v>2.55</v>
       </c>
       <c r="P332">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="Q332">
-        <v>1.775</v>
+        <v>2.125</v>
       </c>
       <c r="R332">
-        <v>2.025</v>
+        <v>1.75</v>
       </c>
       <c r="S332">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="T332">
-        <v>1.775</v>
+        <v>2.05</v>
       </c>
       <c r="U332">
-        <v>2.025</v>
+        <v>1.8</v>
       </c>
       <c r="V332">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W332">
         <v>-1</v>
       </c>
       <c r="X332">
-        <v>-1</v>
+        <v>1.55</v>
       </c>
       <c r="Y332">
-        <v>0.3875</v>
+        <v>-1</v>
       </c>
       <c r="Z332">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AA332">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB332">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="333" spans="1:28">
@@ -29208,7 +29208,7 @@
         <v>331</v>
       </c>
       <c r="B333">
-        <v>6390738</v>
+        <v>7323855</v>
       </c>
       <c r="C333" t="s">
         <v>45</v>
@@ -29217,13 +29217,13 @@
         <v>45215.64583333334</v>
       </c>
       <c r="E333" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F333" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G333">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H333">
         <v>0</v>
@@ -29235,40 +29235,40 @@
         <v>1.909</v>
       </c>
       <c r="K333">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="L333">
+        <v>3.75</v>
+      </c>
+      <c r="M333">
+        <v>2.05</v>
+      </c>
+      <c r="N333">
+        <v>3.2</v>
+      </c>
+      <c r="O333">
         <v>4</v>
       </c>
-      <c r="M333">
-        <v>1.363</v>
-      </c>
-      <c r="N333">
-        <v>4</v>
-      </c>
-      <c r="O333">
-        <v>13</v>
-      </c>
       <c r="P333">
-        <v>-1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q333">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="R333">
-        <v>1.95</v>
+        <v>1.775</v>
       </c>
       <c r="S333">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="T333">
-        <v>1.875</v>
+        <v>1.75</v>
       </c>
       <c r="U333">
-        <v>1.925</v>
+        <v>2.05</v>
       </c>
       <c r="V333">
-        <v>0.363</v>
+        <v>1.05</v>
       </c>
       <c r="W333">
         <v>-1</v>
@@ -29277,16 +29277,16 @@
         <v>-1</v>
       </c>
       <c r="Y333">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="Z333">
         <v>-1</v>
       </c>
       <c r="AA333">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB333">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="334" spans="1:28">
@@ -29294,7 +29294,7 @@
         <v>332</v>
       </c>
       <c r="B334">
-        <v>7323855</v>
+        <v>7323927</v>
       </c>
       <c r="C334" t="s">
         <v>45</v>
@@ -29303,76 +29303,76 @@
         <v>45215.64583333334</v>
       </c>
       <c r="E334" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="F334" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="G334">
         <v>1</v>
       </c>
       <c r="H334">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I334" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J334">
-        <v>1.909</v>
+        <v>4</v>
       </c>
       <c r="K334">
         <v>3.2</v>
       </c>
       <c r="L334">
-        <v>3.75</v>
+        <v>1.8</v>
       </c>
       <c r="M334">
+        <v>3.8</v>
+      </c>
+      <c r="N334">
+        <v>3.3</v>
+      </c>
+      <c r="O334">
         <v>2.05</v>
       </c>
-      <c r="N334">
-        <v>3.2</v>
-      </c>
-      <c r="O334">
-        <v>4</v>
-      </c>
       <c r="P334">
+        <v>0.25</v>
+      </c>
+      <c r="Q334">
+        <v>1.975</v>
+      </c>
+      <c r="R334">
+        <v>1.875</v>
+      </c>
+      <c r="S334">
+        <v>2.25</v>
+      </c>
+      <c r="T334">
+        <v>1.825</v>
+      </c>
+      <c r="U334">
+        <v>2.025</v>
+      </c>
+      <c r="V334">
+        <v>-1</v>
+      </c>
+      <c r="W334">
+        <v>2.3</v>
+      </c>
+      <c r="X334">
+        <v>-1</v>
+      </c>
+      <c r="Y334">
+        <v>0.4875</v>
+      </c>
+      <c r="Z334">
         <v>-0.5</v>
       </c>
-      <c r="Q334">
-        <v>2.025</v>
-      </c>
-      <c r="R334">
-        <v>1.775</v>
-      </c>
-      <c r="S334">
-        <v>1.75</v>
-      </c>
-      <c r="T334">
-        <v>1.75</v>
-      </c>
-      <c r="U334">
-        <v>2.05</v>
-      </c>
-      <c r="V334">
-        <v>1.05</v>
-      </c>
-      <c r="W334">
-        <v>-1</v>
-      </c>
-      <c r="X334">
-        <v>-1</v>
-      </c>
-      <c r="Y334">
-        <v>1.025</v>
-      </c>
-      <c r="Z334">
-        <v>-1</v>
-      </c>
       <c r="AA334">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB334">
-        <v>1.05</v>
+        <v>0.5125</v>
       </c>
     </row>
     <row r="335" spans="1:28">
@@ -29380,7 +29380,7 @@
         <v>333</v>
       </c>
       <c r="B335">
-        <v>7323927</v>
+        <v>7323841</v>
       </c>
       <c r="C335" t="s">
         <v>45</v>
@@ -29389,76 +29389,76 @@
         <v>45215.64583333334</v>
       </c>
       <c r="E335" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="F335" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G335">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H335">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I335" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J335">
-        <v>4</v>
+        <v>2.375</v>
       </c>
       <c r="K335">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="L335">
-        <v>1.8</v>
+        <v>2.75</v>
       </c>
       <c r="M335">
-        <v>3.8</v>
+        <v>2.05</v>
       </c>
       <c r="N335">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="O335">
-        <v>2.05</v>
+        <v>3.75</v>
       </c>
       <c r="P335">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="Q335">
-        <v>1.975</v>
+        <v>1.775</v>
       </c>
       <c r="R335">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="S335">
         <v>2.25</v>
       </c>
       <c r="T335">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="U335">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="V335">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="W335">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="X335">
         <v>-1</v>
       </c>
       <c r="Y335">
-        <v>0.4875</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="Z335">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AA335">
-        <v>-0.5</v>
+        <v>0.95</v>
       </c>
       <c r="AB335">
-        <v>0.5125</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="336" spans="1:28">
@@ -29466,7 +29466,7 @@
         <v>334</v>
       </c>
       <c r="B336">
-        <v>7323841</v>
+        <v>7311908</v>
       </c>
       <c r="C336" t="s">
         <v>45</v>
@@ -29475,73 +29475,73 @@
         <v>45215.64583333334</v>
       </c>
       <c r="E336" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F336" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G336">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H336">
         <v>2</v>
       </c>
       <c r="I336" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J336">
-        <v>2.375</v>
+        <v>2</v>
       </c>
       <c r="K336">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="L336">
-        <v>2.75</v>
+        <v>3.3</v>
       </c>
       <c r="M336">
-        <v>2.05</v>
+        <v>1.8</v>
       </c>
       <c r="N336">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="O336">
+        <v>4.75</v>
+      </c>
+      <c r="P336">
+        <v>-0.75</v>
+      </c>
+      <c r="Q336">
+        <v>1.975</v>
+      </c>
+      <c r="R336">
+        <v>1.825</v>
+      </c>
+      <c r="S336">
+        <v>2</v>
+      </c>
+      <c r="T336">
+        <v>1.925</v>
+      </c>
+      <c r="U336">
+        <v>1.875</v>
+      </c>
+      <c r="V336">
+        <v>-1</v>
+      </c>
+      <c r="W336">
+        <v>-1</v>
+      </c>
+      <c r="X336">
         <v>3.75</v>
       </c>
-      <c r="P336">
-        <v>-0.25</v>
-      </c>
-      <c r="Q336">
-        <v>1.775</v>
-      </c>
-      <c r="R336">
-        <v>2.025</v>
-      </c>
-      <c r="S336">
-        <v>2.25</v>
-      </c>
-      <c r="T336">
-        <v>1.95</v>
-      </c>
-      <c r="U336">
-        <v>1.85</v>
-      </c>
-      <c r="V336">
-        <v>1.05</v>
-      </c>
-      <c r="W336">
-        <v>-1</v>
-      </c>
-      <c r="X336">
-        <v>-1</v>
-      </c>
       <c r="Y336">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z336">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AA336">
-        <v>0.95</v>
+        <v>0.925</v>
       </c>
       <c r="AB336">
         <v>-1</v>
@@ -29552,7 +29552,7 @@
         <v>335</v>
       </c>
       <c r="B337">
-        <v>7311908</v>
+        <v>6390738</v>
       </c>
       <c r="C337" t="s">
         <v>45</v>
@@ -29561,73 +29561,73 @@
         <v>45215.64583333334</v>
       </c>
       <c r="E337" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F337" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G337">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H337">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I337" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J337">
-        <v>2</v>
+        <v>1.909</v>
       </c>
       <c r="K337">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="L337">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="M337">
-        <v>1.8</v>
+        <v>1.363</v>
       </c>
       <c r="N337">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="O337">
-        <v>4.75</v>
+        <v>13</v>
       </c>
       <c r="P337">
-        <v>-0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="Q337">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="R337">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="S337">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="T337">
+        <v>1.875</v>
+      </c>
+      <c r="U337">
         <v>1.925</v>
       </c>
-      <c r="U337">
-        <v>1.875</v>
-      </c>
       <c r="V337">
-        <v>-1</v>
+        <v>0.363</v>
       </c>
       <c r="W337">
         <v>-1</v>
       </c>
       <c r="X337">
-        <v>3.75</v>
+        <v>-1</v>
       </c>
       <c r="Y337">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z337">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA337">
-        <v>0.925</v>
+        <v>0.875</v>
       </c>
       <c r="AB337">
         <v>-1</v>
@@ -46494,7 +46494,7 @@
         <v>532</v>
       </c>
       <c r="B534">
-        <v>7698761</v>
+        <v>7698764</v>
       </c>
       <c r="C534" t="s">
         <v>45</v>
@@ -46503,76 +46503,76 @@
         <v>45388.64583333334</v>
       </c>
       <c r="E534" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F534" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="G534">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H534">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I534" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J534">
-        <v>1.727</v>
+        <v>1.8</v>
       </c>
       <c r="K534">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="L534">
-        <v>4.333</v>
+        <v>4</v>
       </c>
       <c r="M534">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="N534">
         <v>3.1</v>
       </c>
       <c r="O534">
-        <v>4</v>
+        <v>4.333</v>
       </c>
       <c r="P534">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q534">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="R534">
-        <v>2.05</v>
+        <v>1.8</v>
       </c>
       <c r="S534">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="T534">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="U534">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="V534">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="W534">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="X534">
         <v>-1</v>
       </c>
       <c r="Y534">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="Z534">
-        <v>0.5249999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA534">
-        <v>0.4875</v>
+        <v>0</v>
       </c>
       <c r="AB534">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="535" spans="1:28">
@@ -46580,7 +46580,7 @@
         <v>533</v>
       </c>
       <c r="B535">
-        <v>7698764</v>
+        <v>7698761</v>
       </c>
       <c r="C535" t="s">
         <v>45</v>
@@ -46589,76 +46589,76 @@
         <v>45388.64583333334</v>
       </c>
       <c r="E535" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F535" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="G535">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H535">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I535" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J535">
-        <v>1.8</v>
+        <v>1.727</v>
       </c>
       <c r="K535">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L535">
-        <v>4</v>
+        <v>4.333</v>
       </c>
       <c r="M535">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="N535">
         <v>3.1</v>
       </c>
       <c r="O535">
-        <v>4.333</v>
+        <v>4</v>
       </c>
       <c r="P535">
+        <v>-0.25</v>
+      </c>
+      <c r="Q535">
+        <v>1.75</v>
+      </c>
+      <c r="R535">
+        <v>2.05</v>
+      </c>
+      <c r="S535">
+        <v>1.75</v>
+      </c>
+      <c r="T535">
+        <v>1.975</v>
+      </c>
+      <c r="U535">
+        <v>1.825</v>
+      </c>
+      <c r="V535">
+        <v>-1</v>
+      </c>
+      <c r="W535">
+        <v>2.1</v>
+      </c>
+      <c r="X535">
+        <v>-1</v>
+      </c>
+      <c r="Y535">
         <v>-0.5</v>
       </c>
-      <c r="Q535">
-        <v>2</v>
-      </c>
-      <c r="R535">
-        <v>1.8</v>
-      </c>
-      <c r="S535">
-        <v>2</v>
-      </c>
-      <c r="T535">
-        <v>2</v>
-      </c>
-      <c r="U535">
-        <v>1.8</v>
-      </c>
-      <c r="V535">
-        <v>0.95</v>
-      </c>
-      <c r="W535">
-        <v>-1</v>
-      </c>
-      <c r="X535">
-        <v>-1</v>
-      </c>
-      <c r="Y535">
-        <v>1</v>
-      </c>
       <c r="Z535">
-        <v>-1</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AA535">
-        <v>0</v>
+        <v>0.4875</v>
       </c>
       <c r="AB535">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="536" spans="1:28">
@@ -46924,7 +46924,7 @@
         <v>537</v>
       </c>
       <c r="B539">
-        <v>7702194</v>
+        <v>7698755</v>
       </c>
       <c r="C539" t="s">
         <v>45</v>
@@ -46933,73 +46933,73 @@
         <v>45389.64583333334</v>
       </c>
       <c r="E539" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F539" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G539">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H539">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I539" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J539">
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="K539">
-        <v>2.75</v>
+        <v>2.875</v>
       </c>
       <c r="L539">
-        <v>2.9</v>
+        <v>3.5</v>
       </c>
       <c r="M539">
-        <v>2.625</v>
+        <v>2</v>
       </c>
       <c r="N539">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="O539">
-        <v>3.2</v>
+        <v>4.75</v>
       </c>
       <c r="P539">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="Q539">
-        <v>1.725</v>
+        <v>2</v>
       </c>
       <c r="R539">
-        <v>2.075</v>
+        <v>1.8</v>
       </c>
       <c r="S539">
         <v>1.75</v>
       </c>
       <c r="T539">
-        <v>1.75</v>
+        <v>1.825</v>
       </c>
       <c r="U539">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="V539">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W539">
         <v>-1</v>
       </c>
       <c r="X539">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="Y539">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z539">
-        <v>1.075</v>
+        <v>-1</v>
       </c>
       <c r="AA539">
-        <v>0.75</v>
+        <v>0.825</v>
       </c>
       <c r="AB539">
         <v>-1</v>
@@ -47010,7 +47010,7 @@
         <v>538</v>
       </c>
       <c r="B540">
-        <v>7698755</v>
+        <v>7702194</v>
       </c>
       <c r="C540" t="s">
         <v>45</v>
@@ -47019,73 +47019,73 @@
         <v>45389.64583333334</v>
       </c>
       <c r="E540" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F540" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G540">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H540">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I540" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J540">
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="K540">
-        <v>2.875</v>
+        <v>2.75</v>
       </c>
       <c r="L540">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="M540">
-        <v>2</v>
+        <v>2.625</v>
       </c>
       <c r="N540">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="O540">
-        <v>4.75</v>
+        <v>3.2</v>
       </c>
       <c r="P540">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="Q540">
-        <v>2</v>
+        <v>1.725</v>
       </c>
       <c r="R540">
-        <v>1.8</v>
+        <v>2.075</v>
       </c>
       <c r="S540">
         <v>1.75</v>
       </c>
       <c r="T540">
-        <v>1.825</v>
+        <v>1.75</v>
       </c>
       <c r="U540">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="V540">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W540">
         <v>-1</v>
       </c>
       <c r="X540">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="Y540">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z540">
-        <v>-1</v>
+        <v>1.075</v>
       </c>
       <c r="AA540">
-        <v>0.825</v>
+        <v>0.75</v>
       </c>
       <c r="AB540">
         <v>-1</v>
@@ -50278,7 +50278,7 @@
         <v>576</v>
       </c>
       <c r="B578">
-        <v>7698791</v>
+        <v>7702191</v>
       </c>
       <c r="C578" t="s">
         <v>45</v>
@@ -50287,13 +50287,13 @@
         <v>45403.54166666666</v>
       </c>
       <c r="E578" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="F578" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="G578">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H578">
         <v>0</v>
@@ -50302,43 +50302,43 @@
         <v>88</v>
       </c>
       <c r="J578">
-        <v>2.1</v>
+        <v>2.625</v>
       </c>
       <c r="K578">
         <v>2.75</v>
       </c>
       <c r="L578">
-        <v>3.6</v>
+        <v>2.75</v>
       </c>
       <c r="M578">
-        <v>1.727</v>
+        <v>2.3</v>
       </c>
       <c r="N578">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="O578">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="P578">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="Q578">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="R578">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="S578">
         <v>1.75</v>
       </c>
       <c r="T578">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="U578">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V578">
-        <v>0.7270000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="W578">
         <v>-1</v>
@@ -50347,16 +50347,16 @@
         <v>-1</v>
       </c>
       <c r="Y578">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="Z578">
+        <v>-1</v>
+      </c>
+      <c r="AA578">
+        <v>0.45</v>
+      </c>
+      <c r="AB578">
         <v>-0.5</v>
-      </c>
-      <c r="AA578">
-        <v>-1</v>
-      </c>
-      <c r="AB578">
-        <v>1.025</v>
       </c>
     </row>
     <row r="579" spans="1:28">
@@ -50364,7 +50364,7 @@
         <v>577</v>
       </c>
       <c r="B579">
-        <v>7702191</v>
+        <v>7698791</v>
       </c>
       <c r="C579" t="s">
         <v>45</v>
@@ -50373,13 +50373,13 @@
         <v>45403.54166666666</v>
       </c>
       <c r="E579" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F579" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G579">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H579">
         <v>0</v>
@@ -50388,43 +50388,43 @@
         <v>88</v>
       </c>
       <c r="J579">
-        <v>2.625</v>
+        <v>2.1</v>
       </c>
       <c r="K579">
         <v>2.75</v>
       </c>
       <c r="L579">
-        <v>2.75</v>
+        <v>3.6</v>
       </c>
       <c r="M579">
-        <v>2.3</v>
+        <v>1.727</v>
       </c>
       <c r="N579">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="O579">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="P579">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="Q579">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="R579">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="S579">
         <v>1.75</v>
       </c>
       <c r="T579">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="U579">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V579">
-        <v>1.3</v>
+        <v>0.7270000000000001</v>
       </c>
       <c r="W579">
         <v>-1</v>
@@ -50433,16 +50433,16 @@
         <v>-1</v>
       </c>
       <c r="Y579">
-        <v>0.95</v>
+        <v>0.5</v>
       </c>
       <c r="Z579">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AA579">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="AB579">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="580" spans="1:28">
@@ -51826,7 +51826,7 @@
         <v>594</v>
       </c>
       <c r="B596">
-        <v>8133935</v>
+        <v>8133801</v>
       </c>
       <c r="C596" t="s">
         <v>45</v>
@@ -51835,16 +51835,16 @@
         <v>45410.625</v>
       </c>
       <c r="E596" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F596" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="G596">
         <v>2</v>
       </c>
       <c r="H596">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I596" t="s">
         <v>88</v>
@@ -51853,40 +51853,40 @@
         <v>2.75</v>
       </c>
       <c r="K596">
-        <v>2.875</v>
+        <v>2.75</v>
       </c>
       <c r="L596">
-        <v>2.5</v>
+        <v>2.625</v>
       </c>
       <c r="M596">
-        <v>2.3</v>
+        <v>2.55</v>
       </c>
       <c r="N596">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="O596">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="P596">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q596">
-        <v>1.95</v>
+        <v>1.725</v>
       </c>
       <c r="R596">
-        <v>1.85</v>
+        <v>2.075</v>
       </c>
       <c r="S596">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T596">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="U596">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="V596">
-        <v>1.3</v>
+        <v>1.55</v>
       </c>
       <c r="W596">
         <v>-1</v>
@@ -51895,16 +51895,16 @@
         <v>-1</v>
       </c>
       <c r="Y596">
-        <v>0.95</v>
+        <v>0.7250000000000001</v>
       </c>
       <c r="Z596">
         <v>-1</v>
       </c>
       <c r="AA596">
-        <v>0.8500000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="AB596">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="597" spans="1:28">
@@ -51912,7 +51912,7 @@
         <v>595</v>
       </c>
       <c r="B597">
-        <v>8133801</v>
+        <v>8133935</v>
       </c>
       <c r="C597" t="s">
         <v>45</v>
@@ -51921,16 +51921,16 @@
         <v>45410.625</v>
       </c>
       <c r="E597" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="F597" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="G597">
         <v>2</v>
       </c>
       <c r="H597">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I597" t="s">
         <v>88</v>
@@ -51939,40 +51939,40 @@
         <v>2.75</v>
       </c>
       <c r="K597">
-        <v>2.75</v>
+        <v>2.875</v>
       </c>
       <c r="L597">
-        <v>2.625</v>
+        <v>2.5</v>
       </c>
       <c r="M597">
-        <v>2.55</v>
+        <v>2.3</v>
       </c>
       <c r="N597">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="O597">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="P597">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="Q597">
-        <v>1.725</v>
+        <v>1.95</v>
       </c>
       <c r="R597">
-        <v>2.075</v>
+        <v>1.85</v>
       </c>
       <c r="S597">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="T597">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="U597">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="V597">
-        <v>1.55</v>
+        <v>1.3</v>
       </c>
       <c r="W597">
         <v>-1</v>
@@ -51981,16 +51981,16 @@
         <v>-1</v>
       </c>
       <c r="Y597">
-        <v>0.7250000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="Z597">
         <v>-1</v>
       </c>
       <c r="AA597">
-        <v>0.4</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB597">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="598" spans="1:28">
@@ -52864,49 +52864,49 @@
         <v>45</v>
       </c>
       <c r="D608" s="2">
-        <v>45415.875</v>
+        <v>45415.79861111111</v>
       </c>
       <c r="E608" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="F608" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="J608">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="K608">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L608">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M608">
-        <v>1.666</v>
+        <v>1.444</v>
       </c>
       <c r="N608">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O608">
-        <v>5.75</v>
+        <v>9</v>
       </c>
       <c r="P608">
-        <v>-0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="Q608">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="R608">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="S608">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="T608">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="U608">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="V608">
         <v>0</v>
@@ -52929,49 +52929,49 @@
         <v>45</v>
       </c>
       <c r="D609" s="2">
-        <v>45415.88194444445</v>
+        <v>45415.875</v>
       </c>
       <c r="E609" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="F609" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="J609">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="K609">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L609">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M609">
-        <v>1.4</v>
+        <v>1.75</v>
       </c>
       <c r="N609">
-        <v>3.8</v>
+        <v>3.1</v>
       </c>
       <c r="O609">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="P609">
-        <v>-1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="Q609">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="R609">
-        <v>1.775</v>
+        <v>1.85</v>
       </c>
       <c r="S609">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="T609">
+        <v>1.8</v>
+      </c>
+      <c r="U609">
         <v>2.05</v>
-      </c>
-      <c r="U609">
-        <v>1.8</v>
       </c>
       <c r="V609">
         <v>0</v>
@@ -53012,31 +53012,31 @@
         <v>2.75</v>
       </c>
       <c r="M610">
-        <v>2.875</v>
+        <v>2.7</v>
       </c>
       <c r="N610">
-        <v>2.75</v>
+        <v>2.8</v>
       </c>
       <c r="O610">
-        <v>2.625</v>
+        <v>2.8</v>
       </c>
       <c r="P610">
         <v>0</v>
       </c>
       <c r="Q610">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="R610">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="S610">
         <v>2</v>
       </c>
       <c r="T610">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="U610">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V610">
         <v>0</v>
@@ -53080,10 +53080,10 @@
         <v>2</v>
       </c>
       <c r="N611">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="O611">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P611">
         <v>-0.5</v>
@@ -53095,13 +53095,13 @@
         <v>1.8</v>
       </c>
       <c r="S611">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T611">
+        <v>1.825</v>
+      </c>
+      <c r="U611">
         <v>2.025</v>
-      </c>
-      <c r="U611">
-        <v>1.825</v>
       </c>
       <c r="V611">
         <v>0</v>
@@ -53142,31 +53142,31 @@
         <v>4</v>
       </c>
       <c r="M612">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="N612">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="O612">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P612">
         <v>-0.5</v>
       </c>
       <c r="Q612">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="R612">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="S612">
         <v>1.75</v>
       </c>
       <c r="T612">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="U612">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V612">
         <v>0</v>
@@ -53272,7 +53272,7 @@
         <v>2.5</v>
       </c>
       <c r="M614">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="N614">
         <v>2.875</v>
@@ -53284,19 +53284,19 @@
         <v>0.25</v>
       </c>
       <c r="Q614">
-        <v>1.775</v>
+        <v>1.75</v>
       </c>
       <c r="R614">
-        <v>2.1</v>
+        <v>2.125</v>
       </c>
       <c r="S614">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T614">
+        <v>1.8</v>
+      </c>
+      <c r="U614">
         <v>2.05</v>
-      </c>
-      <c r="U614">
-        <v>1.8</v>
       </c>
       <c r="V614">
         <v>0</v>
@@ -53337,22 +53337,22 @@
         <v>2.9</v>
       </c>
       <c r="M615">
-        <v>2.45</v>
+        <v>2.4</v>
       </c>
       <c r="N615">
         <v>2.9</v>
       </c>
       <c r="O615">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="P615">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="Q615">
-        <v>1.775</v>
+        <v>2.125</v>
       </c>
       <c r="R615">
-        <v>2.1</v>
+        <v>1.75</v>
       </c>
       <c r="S615">
         <v>1.75</v>
@@ -53452,46 +53452,46 @@
         <v>45416.66666666666</v>
       </c>
       <c r="E617" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F617" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="J617">
-        <v>2.2</v>
+        <v>1.909</v>
       </c>
       <c r="K617">
-        <v>2.875</v>
+        <v>3</v>
       </c>
       <c r="L617">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="M617">
-        <v>2.05</v>
+        <v>1.909</v>
       </c>
       <c r="N617">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="O617">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="P617">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q617">
-        <v>1.8</v>
+        <v>1.975</v>
       </c>
       <c r="R617">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="S617">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="T617">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="U617">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="V617">
         <v>0</v>
@@ -53544,19 +53544,19 @@
         <v>-0.25</v>
       </c>
       <c r="Q618">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="R618">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="S618">
         <v>1.75</v>
       </c>
       <c r="T618">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="U618">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="V618">
         <v>0</v>
@@ -53597,7 +53597,7 @@
         <v>5</v>
       </c>
       <c r="M619">
-        <v>1.571</v>
+        <v>1.55</v>
       </c>
       <c r="N619">
         <v>3.6</v>
@@ -53609,19 +53609,19 @@
         <v>-0.75</v>
       </c>
       <c r="Q619">
-        <v>1.8</v>
+        <v>1.775</v>
       </c>
       <c r="R619">
-        <v>2.05</v>
+        <v>2.1</v>
       </c>
       <c r="S619">
         <v>2</v>
       </c>
       <c r="T619">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="U619">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V619">
         <v>0</v>
@@ -53683,10 +53683,10 @@
         <v>2</v>
       </c>
       <c r="T620">
-        <v>2.1</v>
+        <v>2.025</v>
       </c>
       <c r="U620">
-        <v>1.775</v>
+        <v>1.825</v>
       </c>
       <c r="V620">
         <v>0</v>
@@ -53727,31 +53727,31 @@
         <v>6</v>
       </c>
       <c r="M621">
-        <v>1.65</v>
+        <v>1.444</v>
       </c>
       <c r="N621">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="O621">
-        <v>5.75</v>
+        <v>9</v>
       </c>
       <c r="P621">
-        <v>-0.75</v>
+        <v>-1</v>
       </c>
       <c r="Q621">
+        <v>1.95</v>
+      </c>
+      <c r="R621">
         <v>1.9</v>
-      </c>
-      <c r="R621">
-        <v>1.95</v>
       </c>
       <c r="S621">
         <v>1.75</v>
       </c>
       <c r="T621">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="U621">
-        <v>2.1</v>
+        <v>1.975</v>
       </c>
       <c r="V621">
         <v>0</v>
@@ -53792,10 +53792,10 @@
         <v>5</v>
       </c>
       <c r="M622">
-        <v>1.6</v>
+        <v>1.615</v>
       </c>
       <c r="N622">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="O622">
         <v>5.25</v>
@@ -53804,10 +53804,10 @@
         <v>-0.75</v>
       </c>
       <c r="Q622">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="R622">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="S622">
         <v>2</v>
@@ -53839,49 +53839,49 @@
         <v>45</v>
       </c>
       <c r="D623" s="2">
-        <v>45417.6875</v>
+        <v>45417.66666666666</v>
       </c>
       <c r="E623" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="F623" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="J623">
-        <v>1.909</v>
+        <v>2.2</v>
       </c>
       <c r="K623">
-        <v>3</v>
+        <v>2.875</v>
       </c>
       <c r="L623">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="M623">
-        <v>1.909</v>
+        <v>2.05</v>
       </c>
       <c r="N623">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="O623">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="P623">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="Q623">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="R623">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="S623">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T623">
+        <v>1.9</v>
+      </c>
+      <c r="U623">
         <v>1.95</v>
-      </c>
-      <c r="U623">
-        <v>1.9</v>
       </c>
       <c r="V623">
         <v>0</v>
@@ -53922,31 +53922,31 @@
         <v>4.5</v>
       </c>
       <c r="M624">
-        <v>1.833</v>
+        <v>1.909</v>
       </c>
       <c r="N624">
         <v>3.2</v>
       </c>
       <c r="O624">
-        <v>4.333</v>
+        <v>4</v>
       </c>
       <c r="P624">
         <v>-0.5</v>
       </c>
       <c r="Q624">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="R624">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="S624">
         <v>2.25</v>
       </c>
       <c r="T624">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="U624">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V624">
         <v>0</v>
@@ -53987,31 +53987,31 @@
         <v>4.5</v>
       </c>
       <c r="M625">
-        <v>1.666</v>
+        <v>1.65</v>
       </c>
       <c r="N625">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="O625">
-        <v>4.75</v>
+        <v>4.5</v>
       </c>
       <c r="P625">
         <v>-0.75</v>
       </c>
       <c r="Q625">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="R625">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="S625">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="T625">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="U625">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="V625">
         <v>0</v>

</xml_diff>